<commit_message>
dataset and directory modified
</commit_message>
<xml_diff>
--- a/dataset/wos-engineering.xlsx
+++ b/dataset/wos-engineering.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5516" uniqueCount="2417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6516" uniqueCount="2850">
   <si>
     <t>Publisher</t>
   </si>
@@ -7325,6 +7325,1305 @@
   </si>
   <si>
     <t>2199-3823 / 2199-3831</t>
+  </si>
+  <si>
+    <t>JOURNAL OF SYMBOLIC COMPUTATION</t>
+  </si>
+  <si>
+    <t>0747-7171 / 1095-855X</t>
+  </si>
+  <si>
+    <t>JOURNAL OF SYSTEMS AND SOFTWARE</t>
+  </si>
+  <si>
+    <t>0164-1212 / 1873-1228</t>
+  </si>
+  <si>
+    <t>JOURNAL OF SYSTEMS ARCHITECTURE</t>
+  </si>
+  <si>
+    <t>1383-7621 / 1873-6165</t>
+  </si>
+  <si>
+    <t>JOURNAL OF TESTING AND EVALUATION</t>
+  </si>
+  <si>
+    <t>0090-3973 / 1945-7553</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE ACM</t>
+  </si>
+  <si>
+    <t>0004-5411 / 1557-735X</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE ACOUSTICAL SOCIETY OF AMERICA</t>
+  </si>
+  <si>
+    <t>ACOUSTICAL SOC AMER AMER INST PHYSICS , STE 1 NO 1, 2 HUNTINGTON QUADRANGLE, MELVILLE, USA, NY, 11747-4502</t>
+  </si>
+  <si>
+    <t>0001-4966 / 1520-8524</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE AIR &amp; WASTE MANAGEMENT ASSOCIATION</t>
+  </si>
+  <si>
+    <t>1096-2247 / 2162-2906</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE AMERICAN CERAMIC SOCIETY</t>
+  </si>
+  <si>
+    <t>0002-7820 / 1551-2916</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE AMERICAN HELICOPTER SOCIETY</t>
+  </si>
+  <si>
+    <t>AMER HELICOPTER SOC INC , 217 N WASHINGTON ST, ALEXANDRIA, USA, VA, 22314</t>
+  </si>
+  <si>
+    <t>0002-8711 / 2161-6027</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE AMERICAN LEATHER CHEMISTS ASSOCIATION</t>
+  </si>
+  <si>
+    <t>AMER LEATHER CHEMISTS ASSOC , 1314 50 ST, STE 103, LUBBOCK, USA, TX, 79412</t>
+  </si>
+  <si>
+    <t>0002-9726</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE AUDIO ENGINEERING SOCIETY</t>
+  </si>
+  <si>
+    <t>AUDIO ENGINEERING SOC , 60 E 42ND ST, NEW YORK, USA, NY, 10165-2520</t>
+  </si>
+  <si>
+    <t>1549-4950</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE AUSTRALIAN CERAMIC SOCIETY</t>
+  </si>
+  <si>
+    <t>2510-1560 / 2510-1579</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE CERAMIC SOCIETY OF JAPAN</t>
+  </si>
+  <si>
+    <t>CERAMIC SOC JAPAN-NIPPON SERAMIKKUSU KYOKAI , 22-17, HYAKUNIN-CHO 2-CHOME, SHINJUKU-KU, TOKYO, JAPAN, 169-0073</t>
+  </si>
+  <si>
+    <t>1882-0743 / 1348-6535</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE CHINESE INSTITUTE OF ENGINEERS</t>
+  </si>
+  <si>
+    <t>0253-3839 / 2158-7299</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE ELECTROCHEMICAL SOCIETY</t>
+  </si>
+  <si>
+    <t>0013-4651 / 1945-7111</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE ENERGY INSTITUTE</t>
+  </si>
+  <si>
+    <t>1743-9671 / 1746-0220</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE EUROPEAN CERAMIC SOCIETY</t>
+  </si>
+  <si>
+    <t>0955-2219 / 1873-619X</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE EUROPEAN OPTICAL SOCIETY-RAPID PUBLICATIONS</t>
+  </si>
+  <si>
+    <t>1990-2573</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE FRANKLIN INSTITUTE-ENGINEERING AND APPLIED MATHEMATICS</t>
+  </si>
+  <si>
+    <t>0016-0032 / 1879-2693</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE JAPAN INSTITUTE OF METALS AND MATERIALS</t>
+  </si>
+  <si>
+    <t>JAPAN INST METALS &amp; MATERIALS , 1-14-32, ICHIBANCHO, AOBA-KU, SENDAI, JAPAN, 980-8544</t>
+  </si>
+  <si>
+    <t>0021-4876 / 1880-6880</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE JAPAN PETROLEUM INSTITUTE</t>
+  </si>
+  <si>
+    <t>JAPAN PETROLEUM INST , YOYU-KANDA BLDG. 4F, 1-8-4 KANDASUDA-CHO, CHIYODA-KU, TOKYO, JAPAN, 108-0041</t>
+  </si>
+  <si>
+    <t>1346-8804 / 1349-273X</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE KOREAN CERAMIC SOCIETY</t>
+  </si>
+  <si>
+    <t>1229-7801 / 2234-0491</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE MECHANICS AND PHYSICS OF SOLIDS</t>
+  </si>
+  <si>
+    <t>0022-5096 / 1873-4782</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE OPERATIONAL RESEARCH SOCIETY</t>
+  </si>
+  <si>
+    <t>0160-5682 / 1476-9360</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE OPTICAL SOCIETY OF AMERICA A-OPTICS IMAGE SCIENCE AND VISION</t>
+  </si>
+  <si>
+    <t>1084-7529 / 1520-8532</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE OPTICAL SOCIETY OF AMERICA B-OPTICAL PHYSICS</t>
+  </si>
+  <si>
+    <t>0740-3224 / 1520-8540</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE SOCIETY FOR INFORMATION DISPLAY</t>
+  </si>
+  <si>
+    <t>1071-0922 / 1938-3657</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE SOCIETY OF LEATHER TECHNOLOGISTS AND CHEMISTS</t>
+  </si>
+  <si>
+    <t>SOC LEATHER TECHNOL CHEMISTS , 8 COPPER LEAF CLOSE, MOULTON, ENGLAND, NORTHAMPTON, NN3 7HS</t>
+  </si>
+  <si>
+    <t>0144-0322</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE SOUTHERN AFRICAN INSTITUTE OF MINING AND METALLURGY</t>
+  </si>
+  <si>
+    <t>SOUTHERN AFRICAN INST MINING METALLURGY , 5 HOLLARD ST, 5TH FLOOR, CHAMBER OF MINES BUILDING, PO BOX 61127, MARSHALLTOWN L, SOUTH AFRICA, 2107</t>
+  </si>
+  <si>
+    <t>2225-6253 / 2411-9717</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THE TAIWAN INSTITUTE OF CHEMICAL ENGINEERS</t>
+  </si>
+  <si>
+    <t>1876-1070 / 1876-1089</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THEORETICAL AND COMPUTATIONAL ACOUSTICS</t>
+  </si>
+  <si>
+    <t>2591-7285 / 2591-7811</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THERMAL SCIENCE AND ENGINEERING APPLICATIONS</t>
+  </si>
+  <si>
+    <t>1948-5085 / 1948-5093</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THERMAL SPRAY TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>1059-9630 / 1544-1016</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THERMAL STRESSES</t>
+  </si>
+  <si>
+    <t>0149-5739 / 1521-074X</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THERMOPHYSICS AND HEAT TRANSFER</t>
+  </si>
+  <si>
+    <t>0887-8722 / 1533-6808</t>
+  </si>
+  <si>
+    <t>JOURNAL OF THERMOPLASTIC COMPOSITE MATERIALS</t>
+  </si>
+  <si>
+    <t>0892-7057 / 1530-7980</t>
+  </si>
+  <si>
+    <t>JOURNAL OF TRANSPORTATION ENGINEERING PART A-SYSTEMS</t>
+  </si>
+  <si>
+    <t>2473-2907 / 2473-2893</t>
+  </si>
+  <si>
+    <t>JOURNAL OF TRANSPORTATION ENGINEERING PART B-PAVEMENTS</t>
+  </si>
+  <si>
+    <t>2573-5438</t>
+  </si>
+  <si>
+    <t>JOURNAL OF TRIBOLOGY-TRANSACTIONS OF THE ASME</t>
+  </si>
+  <si>
+    <t>0742-4787 / 1528-8897</t>
+  </si>
+  <si>
+    <t>JOURNAL OF TURBOMACHINERY-TRANSACTIONS OF THE ASME</t>
+  </si>
+  <si>
+    <t>0889-504X / 1528-8900</t>
+  </si>
+  <si>
+    <t>JOURNAL OF TURBULENCE</t>
+  </si>
+  <si>
+    <t>1468-5248</t>
+  </si>
+  <si>
+    <t>JOURNAL OF UNIVERSAL COMPUTER SCIENCE</t>
+  </si>
+  <si>
+    <t>GRAZ UNIV TECHNOLGOY, INST INFORMATION SYSTEMS COMPUTER MEDIA-IICM , INFFELDGASSE 16C, GRAZ, AUSTRIA, A-8010</t>
+  </si>
+  <si>
+    <t>0948-695X / 0948-6968</t>
+  </si>
+  <si>
+    <t>JOURNAL OF URBAN PLANNING AND DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>0733-9488 / 1943-5444</t>
+  </si>
+  <si>
+    <t>JOURNAL OF VACUUM SCIENCE &amp; TECHNOLOGY A</t>
+  </si>
+  <si>
+    <t>A V S AMER INST PHYSICS , STE 1 NO 1, 2 HUNTINGTON QUADRANGLE, MELVILLE, USA, NY, 11747-4502</t>
+  </si>
+  <si>
+    <t>0734-2101 / 1520-8559</t>
+  </si>
+  <si>
+    <t>JOURNAL OF VACUUM SCIENCE &amp; TECHNOLOGY B</t>
+  </si>
+  <si>
+    <t>2166-2746 / 2166-2754</t>
+  </si>
+  <si>
+    <t>JOURNAL OF VIBRATION AND ACOUSTICS-TRANSACTIONS OF THE ASME</t>
+  </si>
+  <si>
+    <t>1048-9002 / 1528-8927</t>
+  </si>
+  <si>
+    <t>JOURNAL OF VIBRATION AND CONTROL</t>
+  </si>
+  <si>
+    <t>1077-5463 / 1741-2986</t>
+  </si>
+  <si>
+    <t>JOURNAL OF VINYL &amp; ADDITIVE TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>1083-5601 / 1548-0585</t>
+  </si>
+  <si>
+    <t>JOURNAL OF VISUAL COMMUNICATION AND IMAGE REPRESENTATION</t>
+  </si>
+  <si>
+    <t>1047-3203 / 1095-9076</t>
+  </si>
+  <si>
+    <t>JOURNAL OF VISUALIZATION</t>
+  </si>
+  <si>
+    <t>1343-8875 / 1875-8975</t>
+  </si>
+  <si>
+    <t>JOURNAL OF WATER PROCESS ENGINEERING</t>
+  </si>
+  <si>
+    <t>2214-7144</t>
+  </si>
+  <si>
+    <t>JOURNAL OF WATER RESOURCES PLANNING AND MANAGEMENT</t>
+  </si>
+  <si>
+    <t>0733-9496 / 1943-5452</t>
+  </si>
+  <si>
+    <t>JOURNAL OF WATERWAY PORT COASTAL AND OCEAN ENGINEERING</t>
+  </si>
+  <si>
+    <t>0733-950X / 1943-5460</t>
+  </si>
+  <si>
+    <t>JOURNAL OF WEB ENGINEERING</t>
+  </si>
+  <si>
+    <t>RIVER PUBLISHERS , ALSBJERGVEJ 10, GISTRUP, DENMARK, 9260</t>
+  </si>
+  <si>
+    <t>1540-9589 / 1544-5976</t>
+  </si>
+  <si>
+    <t>JOURNAL OF WEB SEMANTICS</t>
+  </si>
+  <si>
+    <t>1570-8268 / 1873-7749</t>
+  </si>
+  <si>
+    <t>JOURNAL OF WOOD CHEMISTRY AND TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>0277-3813 / 1532-2319</t>
+  </si>
+  <si>
+    <t>JOURNAL OF WOOD SCIENCE</t>
+  </si>
+  <si>
+    <t>1435-0211 / 1611-4663</t>
+  </si>
+  <si>
+    <t>JOURNAL ON MULTIMODAL USER INTERFACES</t>
+  </si>
+  <si>
+    <t>1783-7677 / 1783-8738</t>
+  </si>
+  <si>
+    <t>KAGAKU KOGAKU RONBUNSHU</t>
+  </si>
+  <si>
+    <t>0386-216X / 1349-9203</t>
+  </si>
+  <si>
+    <t>KERNTECHNIK</t>
+  </si>
+  <si>
+    <t>0932-3902 / 2195-8580</t>
+  </si>
+  <si>
+    <t>KGK-KAUTSCHUK GUMMI KUNSTSTOFFE</t>
+  </si>
+  <si>
+    <t>DR ALFRED HUTHIG VERLAG GMBH , POSTFACH 10 28 69, HEIDELBERG, GERMANY, D-69018</t>
+  </si>
+  <si>
+    <t>0948-3276</t>
+  </si>
+  <si>
+    <t>KINETICS AND CATALYSIS</t>
+  </si>
+  <si>
+    <t>0023-1584 / 1608-3210</t>
+  </si>
+  <si>
+    <t>KNOWLEDGE AND INFORMATION SYSTEMS</t>
+  </si>
+  <si>
+    <t>0219-1377 / 0219-3116</t>
+  </si>
+  <si>
+    <t>KNOWLEDGE ENGINEERING REVIEW</t>
+  </si>
+  <si>
+    <t>0269-8889 / 1469-8005</t>
+  </si>
+  <si>
+    <t>KONA POWDER AND PARTICLE JOURNAL</t>
+  </si>
+  <si>
+    <t>HOSOKAWA POWDER TECHNOL FOUNDATION , NO 9, 1-CHOME, SHOUDAI TAJIKA, HIRAKATA-SHI, JAPAN, OSAKA, 573-1132</t>
+  </si>
+  <si>
+    <t>0288-4534 / 2187-5537</t>
+  </si>
+  <si>
+    <t>KOREAN JOURNAL OF CHEMICAL ENGINEERING</t>
+  </si>
+  <si>
+    <t>KOREAN INSTITUTE CHEMICAL ENGINEERS , F.5, 119, ANAM-RO, SEONGBUK-GU, SEOUL, SOUTH KOREA, 136-075</t>
+  </si>
+  <si>
+    <t>0256-1115 / 1975-7220</t>
+  </si>
+  <si>
+    <t>KOVOVE MATERIALY-METALLIC MATERIALS</t>
+  </si>
+  <si>
+    <t>REDAKCIA KOVOVE MATERIALY , UL RACIANSKA 75, PO BOX 95, BRATISLAVA 38, SLOVAKIA, 830 08</t>
+  </si>
+  <si>
+    <t>0023-432X / 1338-4252</t>
+  </si>
+  <si>
+    <t>KYBERNETES</t>
+  </si>
+  <si>
+    <t>0368-492X / 1758-7883</t>
+  </si>
+  <si>
+    <t>KYBERNETIKA</t>
+  </si>
+  <si>
+    <t>KYBERNETIKA , POD VODARENSKOU VEZI 4, PRAGUE 8, CZECH REPUBLIC, 182 08</t>
+  </si>
+  <si>
+    <t>0023-5954 / 1805-949X</t>
+  </si>
+  <si>
+    <t>LANDSLIDES</t>
+  </si>
+  <si>
+    <t>1612-510X / 1612-5118</t>
+  </si>
+  <si>
+    <t>LASER FOCUS WORLD</t>
+  </si>
+  <si>
+    <t>PENNWELL PUBL CO , 98 SPIT BROOK RD, NASHUA, USA, NH, 03062-2801</t>
+  </si>
+  <si>
+    <t>1043-8092</t>
+  </si>
+  <si>
+    <t>LASER PHYSICS</t>
+  </si>
+  <si>
+    <t>1054-660X / 1555-6611</t>
+  </si>
+  <si>
+    <t>LATIN AMERICAN APPLIED RESEARCH</t>
+  </si>
+  <si>
+    <t>PLAPIQUI(UNS-CONICET) , CAMINO LA CARRINDANGA, KM 7, C C 717, BAHIA BLANCA, ARGENTINA, 8000</t>
+  </si>
+  <si>
+    <t>0327-0793 / 1851-8796</t>
+  </si>
+  <si>
+    <t>LEUKOS</t>
+  </si>
+  <si>
+    <t>1550-2724 / 1550-2716</t>
+  </si>
+  <si>
+    <t>LIGHT-SCIENCE &amp; APPLICATIONS</t>
+  </si>
+  <si>
+    <t>2047-7538</t>
+  </si>
+  <si>
+    <t>LIGHTING RESEARCH &amp; TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>1477-1535 / 1477-0938</t>
+  </si>
+  <si>
+    <t>LOGICAL METHODS IN COMPUTER SCIENCE</t>
+  </si>
+  <si>
+    <t>LOGICAL METHODS COMPUTER SCIENCE E V , KLEISTSTR 22, BRAUNSCHWEIG, GERMANY, 38124</t>
+  </si>
+  <si>
+    <t>1860-5974</t>
+  </si>
+  <si>
+    <t>LUBRICANTS</t>
+  </si>
+  <si>
+    <t>2075-4442</t>
+  </si>
+  <si>
+    <t>LUBRICATION SCIENCE</t>
+  </si>
+  <si>
+    <t>0954-0075 / 1557-6833</t>
+  </si>
+  <si>
+    <t>MACHINE LEARNING</t>
+  </si>
+  <si>
+    <t>0885-6125 / 1573-0565</t>
+  </si>
+  <si>
+    <t>MACHINE LEARNING-SCIENCE AND TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>2632-2153</t>
+  </si>
+  <si>
+    <t>MACHINE VISION AND APPLICATIONS</t>
+  </si>
+  <si>
+    <t>0932-8092 / 1432-1769</t>
+  </si>
+  <si>
+    <t>MACHINES</t>
+  </si>
+  <si>
+    <t>2075-1702</t>
+  </si>
+  <si>
+    <t>MACHINING SCIENCE AND TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>1091-0344 / 1532-2483</t>
+  </si>
+  <si>
+    <t>MACROMOLECULAR REACTION ENGINEERING</t>
+  </si>
+  <si>
+    <t>1862-832X / 1862-8338</t>
+  </si>
+  <si>
+    <t>MAGAZINE OF CONCRETE RESEARCH</t>
+  </si>
+  <si>
+    <t>0024-9831 / 1751-763X</t>
+  </si>
+  <si>
+    <t>MANUFACTURING ENGINEERING</t>
+  </si>
+  <si>
+    <t>SOC MANUFACTURING ENGINEERS , ONE SME DRIVE, PO BOX 930, DEARBORN, USA, MI, 48121-0930</t>
+  </si>
+  <si>
+    <t>0361-0853</t>
+  </si>
+  <si>
+    <t>MARINE GEORESOURCES &amp; GEOTECHNOLOGY</t>
+  </si>
+  <si>
+    <t>1064-119X / 1521-0618</t>
+  </si>
+  <si>
+    <t>MARINE STRUCTURES</t>
+  </si>
+  <si>
+    <t>0951-8339 / 1873-4170</t>
+  </si>
+  <si>
+    <t>MARINE TECHNOLOGY SOCIETY JOURNAL</t>
+  </si>
+  <si>
+    <t>MARINE TECHNOLOGY SOC INC , 5565 STERRETT PLACE, STE 108, COLUMBIA, USA, MD, 21044</t>
+  </si>
+  <si>
+    <t>0025-3324 / 1948-1209</t>
+  </si>
+  <si>
+    <t>Current Contents Engineering, Computing &amp; Technology | Essential Science Indicators | Zoological Record</t>
+  </si>
+  <si>
+    <t>MATERIALS</t>
+  </si>
+  <si>
+    <t>1996-1944</t>
+  </si>
+  <si>
+    <t>MATERIALS &amp; DESIGN</t>
+  </si>
+  <si>
+    <t>0264-1275 / 1873-4197</t>
+  </si>
+  <si>
+    <t>MATERIALS AND CORROSION-WERKSTOFFE UND KORROSION</t>
+  </si>
+  <si>
+    <t>0947-5117 / 1521-4176</t>
+  </si>
+  <si>
+    <t>MATERIALS AND STRUCTURES</t>
+  </si>
+  <si>
+    <t>1359-5997 / 1871-6873</t>
+  </si>
+  <si>
+    <t>MATERIALS AT HIGH TEMPERATURES</t>
+  </si>
+  <si>
+    <t>0960-3409 / 1878-6413</t>
+  </si>
+  <si>
+    <t>MATERIALS CHARACTERIZATION</t>
+  </si>
+  <si>
+    <t>1044-5803 / 1873-4189</t>
+  </si>
+  <si>
+    <t>MATERIALS CHEMISTRY AND PHYSICS</t>
+  </si>
+  <si>
+    <t>0254-0584 / 1879-3312</t>
+  </si>
+  <si>
+    <t>MATERIALS EVALUATION</t>
+  </si>
+  <si>
+    <t>AMER SOC NONDESTRUCTIVE TEST , 1711 ARLINGATE LANE PO BOX 28518, COLUMBUS, USA, OH, 43228-0518</t>
+  </si>
+  <si>
+    <t>0025-5327</t>
+  </si>
+  <si>
+    <t>JOURNAL OF WIND ENGINEERING AND INDUSTRIAL AERODYNAMICS</t>
+  </si>
+  <si>
+    <t>0167-6105 / 1872-8197</t>
+  </si>
+  <si>
+    <t>KNOWLEDGE-BASED SYSTEMS</t>
+  </si>
+  <si>
+    <t>0950-7051 / 1872-7409</t>
+  </si>
+  <si>
+    <t>MATERIALS EXPRESS</t>
+  </si>
+  <si>
+    <t>2158-5849 / 2158-5857</t>
+  </si>
+  <si>
+    <t>MATERIALS LETTERS</t>
+  </si>
+  <si>
+    <t>0167-577X / 1873-4979</t>
+  </si>
+  <si>
+    <t>MATERIALS PERFORMANCE</t>
+  </si>
+  <si>
+    <t>0094-1492</t>
+  </si>
+  <si>
+    <t>MATERIALS RESEARCH BULLETIN</t>
+  </si>
+  <si>
+    <t>0025-5408 / 1873-4227</t>
+  </si>
+  <si>
+    <t>MATERIALS RESEARCH LETTERS</t>
+  </si>
+  <si>
+    <t>2166-3831</t>
+  </si>
+  <si>
+    <t>MATERIALS SCIENCE AND ENGINEERING A-STRUCTURAL MATERIALS PROPERTIES MICROSTRUCTURE AND PROCESSING</t>
+  </si>
+  <si>
+    <t>0921-5093 / 1873-4936</t>
+  </si>
+  <si>
+    <t>MATERIALS SCIENCE AND ENGINEERING B-ADVANCED FUNCTIONAL SOLID-STATE MATERIALS</t>
+  </si>
+  <si>
+    <t>0921-5107 / 1873-4944</t>
+  </si>
+  <si>
+    <t>MATERIALS SCIENCE AND TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>0267-0836 / 1743-2847</t>
+  </si>
+  <si>
+    <t>MATERIALS SCIENCE IN SEMICONDUCTOR PROCESSING</t>
+  </si>
+  <si>
+    <t>1369-8001 / 1873-4081</t>
+  </si>
+  <si>
+    <t>MATERIALS TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>1066-7857 / 1753-5557</t>
+  </si>
+  <si>
+    <t>MATERIALS TODAY ADVANCES</t>
+  </si>
+  <si>
+    <t>2590-0498</t>
+  </si>
+  <si>
+    <t>MATERIALS TODAY BIO</t>
+  </si>
+  <si>
+    <t>2590-0064</t>
+  </si>
+  <si>
+    <t>MATERIALS TODAY CHEMISTRY</t>
+  </si>
+  <si>
+    <t>2468-5194</t>
+  </si>
+  <si>
+    <t>MATERIALS TODAY ENERGY</t>
+  </si>
+  <si>
+    <t>2468-6069</t>
+  </si>
+  <si>
+    <t>MATERIALS TODAY NANO</t>
+  </si>
+  <si>
+    <t>2588-8420</t>
+  </si>
+  <si>
+    <t>MATERIALS TODAY SUSTAINABILITY</t>
+  </si>
+  <si>
+    <t>2589-2347</t>
+  </si>
+  <si>
+    <t>MATERIALS TRANSACTIONS</t>
+  </si>
+  <si>
+    <t>1345-9678 / 1347-5320</t>
+  </si>
+  <si>
+    <t>MATERIALWISSENSCHAFT UND WERKSTOFFTECHNIK</t>
+  </si>
+  <si>
+    <t>0933-5137 / 1521-4052</t>
+  </si>
+  <si>
+    <t>MATHEMATICAL AND COMPUTER MODELLING OF DYNAMICAL SYSTEMS</t>
+  </si>
+  <si>
+    <t>1387-3954 / 1744-5051</t>
+  </si>
+  <si>
+    <t>MATHEMATICAL METHODS OF OPERATIONS RESEARCH</t>
+  </si>
+  <si>
+    <t>1432-2994 / 1432-5217</t>
+  </si>
+  <si>
+    <t>MATHEMATICAL PROBLEMS IN ENGINEERING</t>
+  </si>
+  <si>
+    <t>1024-123X / 1563-5147</t>
+  </si>
+  <si>
+    <t>MATHEMATICAL PROGRAMMING COMPUTATION</t>
+  </si>
+  <si>
+    <t>1867-2949 / 1867-2957</t>
+  </si>
+  <si>
+    <t>MATHEMATICAL STRUCTURES IN COMPUTER SCIENCE</t>
+  </si>
+  <si>
+    <t>0960-1295 / 1469-8072</t>
+  </si>
+  <si>
+    <t>MATHEMATICS AND COMPUTERS IN SIMULATION</t>
+  </si>
+  <si>
+    <t>0378-4754 / 1872-7166</t>
+  </si>
+  <si>
+    <t>MATHEMATICS AND MECHANICS OF SOLIDS</t>
+  </si>
+  <si>
+    <t>1081-2865 / 1741-3028</t>
+  </si>
+  <si>
+    <t>MATHEMATICS IN ENGINEERING</t>
+  </si>
+  <si>
+    <t>2640-3501</t>
+  </si>
+  <si>
+    <t>MATHEMATICS OF CONTROL SIGNALS AND SYSTEMS</t>
+  </si>
+  <si>
+    <t>0932-4194 / 1435-568X</t>
+  </si>
+  <si>
+    <t>MATTER</t>
+  </si>
+  <si>
+    <t>2590-2393 / 2590-2385</t>
+  </si>
+  <si>
+    <t>MEASUREMENT</t>
+  </si>
+  <si>
+    <t>0263-2241 / 1873-412X</t>
+  </si>
+  <si>
+    <t>MEASUREMENT SCIENCE REVIEW</t>
+  </si>
+  <si>
+    <t>1335-8871</t>
+  </si>
+  <si>
+    <t>MECCANICA</t>
+  </si>
+  <si>
+    <t>0025-6455 / 1572-9648</t>
+  </si>
+  <si>
+    <t>MECHANICAL ENGINEERING</t>
+  </si>
+  <si>
+    <t>0025-6501 / 1943-5649</t>
+  </si>
+  <si>
+    <t>MECHANICAL SCIENCES</t>
+  </si>
+  <si>
+    <t>COPERNICUS GESELLSCHAFT MBH , BAHNHOFSALLEE 1E, GOTTINGEN, GERMANY, 37081</t>
+  </si>
+  <si>
+    <t>2191-9151 / 2191-916X</t>
+  </si>
+  <si>
+    <t>MECHANICAL SYSTEMS AND SIGNAL PROCESSING</t>
+  </si>
+  <si>
+    <t>0888-3270 / 1096-1216</t>
+  </si>
+  <si>
+    <t>MECHANICS BASED DESIGN OF STRUCTURES AND MACHINES</t>
+  </si>
+  <si>
+    <t>1539-7734 / 1539-7742</t>
+  </si>
+  <si>
+    <t>MECHANICS OF COMPOSITE MATERIALS</t>
+  </si>
+  <si>
+    <t>0191-5665 / 1573-8922</t>
+  </si>
+  <si>
+    <t>MECHANICS OF MATERIALS</t>
+  </si>
+  <si>
+    <t>0167-6636 / 1872-7743</t>
+  </si>
+  <si>
+    <t>MECHANICS OF TIME-DEPENDENT MATERIALS</t>
+  </si>
+  <si>
+    <t>1385-2000 / 1573-2738</t>
+  </si>
+  <si>
+    <t>MECHANICS RESEARCH COMMUNICATIONS</t>
+  </si>
+  <si>
+    <t>0093-6413 / 1873-3972</t>
+  </si>
+  <si>
+    <t>MECHANISM AND MACHINE THEORY</t>
+  </si>
+  <si>
+    <t>0094-114X / 1873-3999</t>
+  </si>
+  <si>
+    <t>MECHATRONICS</t>
+  </si>
+  <si>
+    <t>0957-4158</t>
+  </si>
+  <si>
+    <t>MEDICAL &amp; BIOLOGICAL ENGINEERING &amp; COMPUTING</t>
+  </si>
+  <si>
+    <t>0140-0118 / 1741-0444</t>
+  </si>
+  <si>
+    <t>MEDICAL IMAGE ANALYSIS</t>
+  </si>
+  <si>
+    <t>1361-8415 / 1361-8423</t>
+  </si>
+  <si>
+    <t>MEMBRANE AND WATER TREATMENT</t>
+  </si>
+  <si>
+    <t>2005-8624 / 2092-7037</t>
+  </si>
+  <si>
+    <t>MEMBRANES</t>
+  </si>
+  <si>
+    <t>2077-0375</t>
+  </si>
+  <si>
+    <t>MEMETIC COMPUTING</t>
+  </si>
+  <si>
+    <t>1865-9284 / 1865-9292</t>
+  </si>
+  <si>
+    <t>METALLURGICAL AND MATERIALS TRANSACTIONS A-PHYSICAL METALLURGY AND MATERIALS SCIENCE</t>
+  </si>
+  <si>
+    <t>1073-5623 / 1543-1940</t>
+  </si>
+  <si>
+    <t>METALLURGICAL AND MATERIALS TRANSACTIONS B-PROCESS METALLURGY AND MATERIALS PROCESSING SCIENCE</t>
+  </si>
+  <si>
+    <t>1073-5615 / 1543-1916</t>
+  </si>
+  <si>
+    <t>METALLURGICAL RESEARCH &amp; TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>2271-3646 / 2271-3654</t>
+  </si>
+  <si>
+    <t>MEASUREMENT SCIENCE AND TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>0957-0233 / 1361-6501</t>
+  </si>
+  <si>
+    <t>M&amp;SOM-MANUFACTURING &amp; SERVICE OPERATIONS MANAGEMENT</t>
+  </si>
+  <si>
+    <t>1523-4614 / 1526-5498</t>
+  </si>
+  <si>
+    <t>METAL SCIENCE AND HEAT TREATMENT</t>
+  </si>
+  <si>
+    <t>0026-0673 / 1573-8973</t>
+  </si>
+  <si>
+    <t>METALLURGIST</t>
+  </si>
+  <si>
+    <t>0026-0894 / 1573-8892</t>
+  </si>
+  <si>
+    <t>METALS</t>
+  </si>
+  <si>
+    <t>2075-4701</t>
+  </si>
+  <si>
+    <t>METALS AND MATERIALS INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>KOREAN INST METALS MATERIALS , KIM BLDG 6TH FLOOR, SEOCHO-DAERO 56 GIL 38, SEOCHO-GU, SEOUL, SOUTH KOREA, 137-881</t>
+  </si>
+  <si>
+    <t>1598-9623 / 2005-4149</t>
+  </si>
+  <si>
+    <t>METROLOGIA</t>
+  </si>
+  <si>
+    <t>0026-1394 / 1681-7575</t>
+  </si>
+  <si>
+    <t>MICRO &amp; NANO LETTERS</t>
+  </si>
+  <si>
+    <t>1750-0443</t>
+  </si>
+  <si>
+    <t>MICROELECTRONIC ENGINEERING</t>
+  </si>
+  <si>
+    <t>0167-9317 / 1873-5568</t>
+  </si>
+  <si>
+    <t>MICROELECTRONICS INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>1356-5362 / 1758-812X</t>
+  </si>
+  <si>
+    <t>MICROELECTRONICS JOURNAL</t>
+  </si>
+  <si>
+    <t>0026-2692 / 1879-2391</t>
+  </si>
+  <si>
+    <t>MICROELECTRONICS RELIABILITY</t>
+  </si>
+  <si>
+    <t>0026-2714 / 1872-941X</t>
+  </si>
+  <si>
+    <t>MICROFLUIDICS AND NANOFLUIDICS</t>
+  </si>
+  <si>
+    <t>1613-4982 / 1613-4990</t>
+  </si>
+  <si>
+    <t>MICROGRAVITY SCIENCE AND TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>0938-0108 / 1875-0494</t>
+  </si>
+  <si>
+    <t>MICROMACHINES</t>
+  </si>
+  <si>
+    <t>2072-666X</t>
+  </si>
+  <si>
+    <t>MICROPROCESSORS AND MICROSYSTEMS</t>
+  </si>
+  <si>
+    <t>0141-9331 / 1872-9436</t>
+  </si>
+  <si>
+    <t>MICROSYSTEM TECHNOLOGIES-MICRO-AND NANOSYSTEMS-INFORMATION STORAGE AND PROCESSING SYSTEMS</t>
+  </si>
+  <si>
+    <t>0946-7076 / 1432-1858</t>
+  </si>
+  <si>
+    <t>MICROSYSTEMS &amp; NANOENGINEERING</t>
+  </si>
+  <si>
+    <t>2055-7434</t>
+  </si>
+  <si>
+    <t>MICROWAVE AND OPTICAL TECHNOLOGY LETTERS</t>
+  </si>
+  <si>
+    <t>0895-2477 / 1098-2760</t>
+  </si>
+  <si>
+    <t>MICROWAVE JOURNAL</t>
+  </si>
+  <si>
+    <t>HORIZON HOUSE PUBLICATIONS INC , 685 CANTON ST, NORWOOD, USA, MA, 02062</t>
+  </si>
+  <si>
+    <t>0192-6225</t>
+  </si>
+  <si>
+    <t>MINERAL PROCESSING AND EXTRACTIVE METALLURGY REVIEW</t>
+  </si>
+  <si>
+    <t>0882-7508 / 1547-7401</t>
+  </si>
+  <si>
+    <t>MINERALS ENGINEERING</t>
+  </si>
+  <si>
+    <t>0892-6875</t>
+  </si>
+  <si>
+    <t>MINING METALLURGY &amp; EXPLORATION</t>
+  </si>
+  <si>
+    <t>2524-3462 / 2524-3470</t>
+  </si>
+  <si>
+    <t>MIT TECHNOLOGY REVIEW</t>
+  </si>
+  <si>
+    <t>TECHNOL REV , 1 MAIN ST, 13 FLR, CAMBRIDGE, USA, MA, 02142</t>
+  </si>
+  <si>
+    <t>1099-274X</t>
+  </si>
+  <si>
+    <t>BIOSIS Previews | BIOSIS Reviews Reports And Meetings | Current Contents Electronics &amp; Telecommunications Collection | Current Contents Engineering, Computing &amp; Technology | Essential Science Indicators</t>
+  </si>
+  <si>
+    <t>MOBILE INFORMATION SYSTEMS</t>
+  </si>
+  <si>
+    <t>1574-017X / 1875-905X</t>
+  </si>
+  <si>
+    <t>MOBILE NETWORKS &amp; APPLICATIONS</t>
+  </si>
+  <si>
+    <t>1383-469X / 1572-8153</t>
+  </si>
+  <si>
+    <t>MODELING IDENTIFICATION AND CONTROL</t>
+  </si>
+  <si>
+    <t>MIC , DIV ENG CYBERNETICS, TRONDHEIM, NORWAY, 7034</t>
+  </si>
+  <si>
+    <t>0332-7353 / 1890-1328</t>
+  </si>
+  <si>
+    <t>MODELLING AND SIMULATION IN MATERIALS SCIENCE AND ENGINEERING</t>
+  </si>
+  <si>
+    <t>0965-0393 / 1361-651X</t>
+  </si>
+  <si>
+    <t>MOKUZAI GAKKAISHI</t>
+  </si>
+  <si>
+    <t>JAPAN WOOD RES SOC , 1-1-17, MUKOGAOKA, BUNKYO-KU, TOKYO, JAPAN, 113-0023</t>
+  </si>
+  <si>
+    <t>0021-4795 / 1880-7577</t>
+  </si>
+  <si>
+    <t>MOLECULAR SYSTEMS DESIGN &amp; ENGINEERING</t>
+  </si>
+  <si>
+    <t>2058-9689</t>
+  </si>
+  <si>
+    <t>MRS BULLETIN</t>
+  </si>
+  <si>
+    <t>0883-7694 / 1938-1425</t>
+  </si>
+  <si>
+    <t>MULTIBODY SYSTEM DYNAMICS</t>
+  </si>
+  <si>
+    <t>1384-5640 / 1573-272X</t>
+  </si>
+  <si>
+    <t>MULTIDIMENSIONAL SYSTEMS AND SIGNAL PROCESSING</t>
+  </si>
+  <si>
+    <t>0923-6082 / 1573-0824</t>
+  </si>
+  <si>
+    <t>MULTIDISCIPLINE MODELING IN MATERIALS AND STRUCTURES</t>
+  </si>
+  <si>
+    <t>1573-6105 / 1573-6113</t>
+  </si>
+  <si>
+    <t>MULTIMEDIA SYSTEMS</t>
+  </si>
+  <si>
+    <t>0942-4962 / 1432-1882</t>
+  </si>
+  <si>
+    <t>MULTIMEDIA TOOLS AND APPLICATIONS</t>
+  </si>
+  <si>
+    <t>1380-7501 / 1573-7721</t>
+  </si>
+  <si>
+    <t>NANO COMMUNICATION NETWORKS</t>
+  </si>
+  <si>
+    <t>1878-7789 / 1878-7797</t>
+  </si>
+  <si>
+    <t>NANO CONVERGENCE</t>
+  </si>
+  <si>
+    <t>2196-5404</t>
+  </si>
+  <si>
+    <t>NANO ENERGY</t>
+  </si>
+  <si>
+    <t>2211-2855 / 2211-3282</t>
+  </si>
+  <si>
+    <t>NANO FUTURES</t>
+  </si>
+  <si>
+    <t>2399-1984</t>
+  </si>
+  <si>
+    <t>NANO RESEARCH</t>
+  </si>
+  <si>
+    <t>1998-0124 / 1998-0000</t>
+  </si>
+  <si>
+    <t>NANOCOMPOSITES</t>
+  </si>
+  <si>
+    <t>2055-0324 / 2055-0332</t>
+  </si>
+  <si>
+    <t>NANOPHOTONICS</t>
+  </si>
+  <si>
+    <t>2192-8606 / 2192-8614</t>
+  </si>
+  <si>
+    <t>NANOSCALE ADVANCES</t>
+  </si>
+  <si>
+    <t>2516-0230</t>
+  </si>
+  <si>
+    <t>NANOSCALE AND MICROSCALE THERMOPHYSICAL ENGINEERING</t>
+  </si>
+  <si>
+    <t>1556-7265 / 1556-7273</t>
+  </si>
+  <si>
+    <t>NANOSCALE HORIZONS</t>
+  </si>
+  <si>
+    <t>2055-6756 / 2055-6764</t>
+  </si>
+  <si>
+    <t>NANOTECHNOLOGY</t>
+  </si>
+  <si>
+    <t>0957-4484 / 1361-6528</t>
+  </si>
+  <si>
+    <t>NATURAL COMPUTING</t>
+  </si>
+  <si>
+    <t>1567-7818 / 1572-9796</t>
+  </si>
+  <si>
+    <t>NATURAL HAZARDS REVIEW</t>
+  </si>
+  <si>
+    <t>1527-6988 / 1527-6996</t>
+  </si>
+  <si>
+    <t>Current Contents Engineering, Computing &amp; Technology | Current Contents Physical, Chemical &amp; Earth Sciences | Current Contents Social And Behavioral Sciences | Essential Science Indicators</t>
+  </si>
+  <si>
+    <t>NATURAL LANGUAGE ENGINEERING</t>
+  </si>
+  <si>
+    <t>1351-3249 / 1469-8110</t>
+  </si>
+  <si>
+    <t>NATURE ELECTRONICS</t>
+  </si>
+  <si>
+    <t>NATURE PORTFOLIO , HEIDELBERGER PLATZ 3, BERLIN, Germany, 14197</t>
+  </si>
+  <si>
+    <t>2520-1131</t>
   </si>
 </sst>
 </file>
@@ -7661,15 +8960,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1101"/>
+  <dimension ref="A1:G1301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1081" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1103" sqref="B1103"/>
+    <sheetView tabSelected="1" topLeftCell="A1172" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A1251" sqref="A1251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="48.42578125" customWidth="1"/>
@@ -27216,6 +28515,3406 @@
         <v>132</v>
       </c>
       <c r="E1101" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:5">
+      <c r="A1102" t="s">
+        <v>2417</v>
+      </c>
+      <c r="B1102" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C1102" t="s">
+        <v>2418</v>
+      </c>
+      <c r="D1102" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1102" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:5">
+      <c r="A1103" t="s">
+        <v>2419</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>2420</v>
+      </c>
+      <c r="D1103" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1103" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:5">
+      <c r="A1104" t="s">
+        <v>2421</v>
+      </c>
+      <c r="B1104" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1104" t="s">
+        <v>2422</v>
+      </c>
+      <c r="D1104" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1104" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:5">
+      <c r="A1105" t="s">
+        <v>2423</v>
+      </c>
+      <c r="B1105" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C1105" t="s">
+        <v>2424</v>
+      </c>
+      <c r="D1105" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1105" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:5">
+      <c r="A1106" t="s">
+        <v>2425</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>2426</v>
+      </c>
+      <c r="D1106" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1106" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:5">
+      <c r="A1107" t="s">
+        <v>2427</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>2429</v>
+      </c>
+      <c r="D1107" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1107" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:5">
+      <c r="A1108" t="s">
+        <v>2430</v>
+      </c>
+      <c r="B1108" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1108" t="s">
+        <v>2431</v>
+      </c>
+      <c r="D1108" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1108" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:5">
+      <c r="A1109" t="s">
+        <v>2432</v>
+      </c>
+      <c r="B1109" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1109" t="s">
+        <v>2433</v>
+      </c>
+      <c r="D1109" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1109" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:5">
+      <c r="A1110" t="s">
+        <v>2434</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>2435</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>2436</v>
+      </c>
+      <c r="D1110" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1110" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:5">
+      <c r="A1111" t="s">
+        <v>2437</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>2438</v>
+      </c>
+      <c r="C1111" t="s">
+        <v>2439</v>
+      </c>
+      <c r="D1111" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1111" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:5">
+      <c r="A1112" t="s">
+        <v>2440</v>
+      </c>
+      <c r="B1112" t="s">
+        <v>2441</v>
+      </c>
+      <c r="C1112" t="s">
+        <v>2442</v>
+      </c>
+      <c r="D1112" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1112" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:5">
+      <c r="A1113" t="s">
+        <v>2443</v>
+      </c>
+      <c r="B1113" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1113" t="s">
+        <v>2444</v>
+      </c>
+      <c r="D1113" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1113" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:5">
+      <c r="A1114" t="s">
+        <v>2445</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>2446</v>
+      </c>
+      <c r="C1114" t="s">
+        <v>2447</v>
+      </c>
+      <c r="D1114" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1114" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:5">
+      <c r="A1115" t="s">
+        <v>2448</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1115" t="s">
+        <v>2449</v>
+      </c>
+      <c r="D1115" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1115" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:5">
+      <c r="A1116" t="s">
+        <v>2450</v>
+      </c>
+      <c r="B1116" t="s">
+        <v>787</v>
+      </c>
+      <c r="C1116" t="s">
+        <v>2451</v>
+      </c>
+      <c r="D1116" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1116" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:5">
+      <c r="A1117" t="s">
+        <v>2452</v>
+      </c>
+      <c r="B1117" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1117" t="s">
+        <v>2453</v>
+      </c>
+      <c r="D1117" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1117" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:5">
+      <c r="A1118" t="s">
+        <v>2454</v>
+      </c>
+      <c r="B1118" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1118" t="s">
+        <v>2455</v>
+      </c>
+      <c r="D1118" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1118" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:5">
+      <c r="A1119" t="s">
+        <v>2456</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1119" t="s">
+        <v>2457</v>
+      </c>
+      <c r="D1119" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1119" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:5">
+      <c r="A1120" t="s">
+        <v>2458</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1120" t="s">
+        <v>2459</v>
+      </c>
+      <c r="D1120" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1120" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:5">
+      <c r="A1121" t="s">
+        <v>2460</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>2461</v>
+      </c>
+      <c r="C1121" t="s">
+        <v>2462</v>
+      </c>
+      <c r="D1121" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1121" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:5">
+      <c r="A1122" t="s">
+        <v>2463</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>2464</v>
+      </c>
+      <c r="C1122" t="s">
+        <v>2465</v>
+      </c>
+      <c r="D1122" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1122" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:5">
+      <c r="A1123" t="s">
+        <v>2466</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1123" t="s">
+        <v>2467</v>
+      </c>
+      <c r="D1123" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1123" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:5">
+      <c r="A1124" t="s">
+        <v>2468</v>
+      </c>
+      <c r="B1124" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1124" t="s">
+        <v>2469</v>
+      </c>
+      <c r="D1124" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1124" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:5">
+      <c r="A1125" t="s">
+        <v>2470</v>
+      </c>
+      <c r="B1125" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1125" t="s">
+        <v>2471</v>
+      </c>
+      <c r="D1125" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1125" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:5">
+      <c r="A1126" t="s">
+        <v>2472</v>
+      </c>
+      <c r="B1126" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1126" t="s">
+        <v>2473</v>
+      </c>
+      <c r="D1126" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1126" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:5">
+      <c r="A1127" t="s">
+        <v>2474</v>
+      </c>
+      <c r="B1127" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1127" t="s">
+        <v>2475</v>
+      </c>
+      <c r="D1127" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1127" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:5">
+      <c r="A1128" t="s">
+        <v>2476</v>
+      </c>
+      <c r="B1128" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1128" t="s">
+        <v>2477</v>
+      </c>
+      <c r="D1128" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1128" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:5">
+      <c r="A1129" t="s">
+        <v>2478</v>
+      </c>
+      <c r="B1129" t="s">
+        <v>2479</v>
+      </c>
+      <c r="C1129" t="s">
+        <v>2480</v>
+      </c>
+      <c r="D1129" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1129" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:5">
+      <c r="A1130" t="s">
+        <v>2481</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>2482</v>
+      </c>
+      <c r="C1130" t="s">
+        <v>2483</v>
+      </c>
+      <c r="D1130" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1130" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:5">
+      <c r="A1131" t="s">
+        <v>2484</v>
+      </c>
+      <c r="B1131" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1131" t="s">
+        <v>2485</v>
+      </c>
+      <c r="D1131" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1131" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:5">
+      <c r="A1132" t="s">
+        <v>2486</v>
+      </c>
+      <c r="B1132" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C1132" t="s">
+        <v>2487</v>
+      </c>
+      <c r="D1132" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1132" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:5">
+      <c r="A1133" t="s">
+        <v>2488</v>
+      </c>
+      <c r="B1133" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1133" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D1133" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1133" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:5">
+      <c r="A1134" t="s">
+        <v>2490</v>
+      </c>
+      <c r="B1134" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1134" t="s">
+        <v>2491</v>
+      </c>
+      <c r="D1134" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1134" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:5">
+      <c r="A1135" t="s">
+        <v>2492</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1135" t="s">
+        <v>2493</v>
+      </c>
+      <c r="D1135" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1135" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:5">
+      <c r="A1136" t="s">
+        <v>2494</v>
+      </c>
+      <c r="B1136" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1136" t="s">
+        <v>2495</v>
+      </c>
+      <c r="D1136" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1136" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:5">
+      <c r="A1137" t="s">
+        <v>2496</v>
+      </c>
+      <c r="B1137" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1137" t="s">
+        <v>2497</v>
+      </c>
+      <c r="D1137" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1137" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:5">
+      <c r="A1138" t="s">
+        <v>2498</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1138" t="s">
+        <v>2499</v>
+      </c>
+      <c r="D1138" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1138" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:5">
+      <c r="A1139" t="s">
+        <v>2500</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1139" t="s">
+        <v>2501</v>
+      </c>
+      <c r="D1139" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1139" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:5">
+      <c r="A1140" t="s">
+        <v>2502</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1140" t="s">
+        <v>2503</v>
+      </c>
+      <c r="D1140" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1140" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:5">
+      <c r="A1141" t="s">
+        <v>2504</v>
+      </c>
+      <c r="B1141" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1141" t="s">
+        <v>2505</v>
+      </c>
+      <c r="D1141" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1141" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:5">
+      <c r="A1142" t="s">
+        <v>2506</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1142" t="s">
+        <v>2507</v>
+      </c>
+      <c r="D1142" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1142" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:5">
+      <c r="A1143" t="s">
+        <v>2508</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>2509</v>
+      </c>
+      <c r="C1143" t="s">
+        <v>2510</v>
+      </c>
+      <c r="D1143" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1143" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:5">
+      <c r="A1144" t="s">
+        <v>2511</v>
+      </c>
+      <c r="B1144" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1144" t="s">
+        <v>2512</v>
+      </c>
+      <c r="D1144" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1144" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:5">
+      <c r="A1145" t="s">
+        <v>2513</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>2514</v>
+      </c>
+      <c r="C1145" t="s">
+        <v>2515</v>
+      </c>
+      <c r="D1145" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1145" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:5">
+      <c r="A1146" t="s">
+        <v>2516</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>2514</v>
+      </c>
+      <c r="C1146" t="s">
+        <v>2517</v>
+      </c>
+      <c r="D1146" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1146" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:5">
+      <c r="A1147" t="s">
+        <v>2518</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1147" t="s">
+        <v>2519</v>
+      </c>
+      <c r="D1147" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1147" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:5">
+      <c r="A1148" t="s">
+        <v>2520</v>
+      </c>
+      <c r="B1148" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1148" t="s">
+        <v>2521</v>
+      </c>
+      <c r="D1148" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1148" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:5">
+      <c r="A1149" t="s">
+        <v>2522</v>
+      </c>
+      <c r="B1149" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1149" t="s">
+        <v>2523</v>
+      </c>
+      <c r="D1149" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1149" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:5">
+      <c r="A1150" t="s">
+        <v>2524</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1150" t="s">
+        <v>2525</v>
+      </c>
+      <c r="D1150" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1150" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:5">
+      <c r="A1151" t="s">
+        <v>2526</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1151" t="s">
+        <v>2527</v>
+      </c>
+      <c r="D1151" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1151" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:5">
+      <c r="A1152" t="s">
+        <v>2528</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1152" t="s">
+        <v>2529</v>
+      </c>
+      <c r="D1152" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1152" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:5">
+      <c r="A1153" t="s">
+        <v>2530</v>
+      </c>
+      <c r="B1153" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1153" t="s">
+        <v>2531</v>
+      </c>
+      <c r="D1153" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1153" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:5">
+      <c r="A1154" t="s">
+        <v>2532</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>2533</v>
+      </c>
+      <c r="D1154" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1154" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:5">
+      <c r="A1155" t="s">
+        <v>2534</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>2535</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>2536</v>
+      </c>
+      <c r="D1155" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1155" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:5">
+      <c r="A1156" t="s">
+        <v>2537</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1156" t="s">
+        <v>2538</v>
+      </c>
+      <c r="D1156" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1156" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:5">
+      <c r="A1157" t="s">
+        <v>2539</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1157" t="s">
+        <v>2540</v>
+      </c>
+      <c r="D1157" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1157" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:5">
+      <c r="A1158" t="s">
+        <v>2541</v>
+      </c>
+      <c r="B1158" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1158" t="s">
+        <v>2542</v>
+      </c>
+      <c r="D1158" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1158" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:5">
+      <c r="A1159" t="s">
+        <v>2543</v>
+      </c>
+      <c r="B1159" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1159" t="s">
+        <v>2544</v>
+      </c>
+      <c r="D1159" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1159" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:5">
+      <c r="A1160" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B1160" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1160" t="s">
+        <v>2546</v>
+      </c>
+      <c r="D1160" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1160" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:5">
+      <c r="A1161" t="s">
+        <v>2547</v>
+      </c>
+      <c r="B1161" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C1161" t="s">
+        <v>2548</v>
+      </c>
+      <c r="D1161" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1161" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:5">
+      <c r="A1162" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>2550</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>2551</v>
+      </c>
+      <c r="D1162" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1162" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:5">
+      <c r="A1163" t="s">
+        <v>2552</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>2553</v>
+      </c>
+      <c r="D1163" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1163" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:5">
+      <c r="A1164" t="s">
+        <v>2554</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>573</v>
+      </c>
+      <c r="C1164" t="s">
+        <v>2555</v>
+      </c>
+      <c r="D1164" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1164" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:5">
+      <c r="A1165" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>953</v>
+      </c>
+      <c r="C1165" t="s">
+        <v>2557</v>
+      </c>
+      <c r="D1165" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1165" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:5">
+      <c r="A1166" t="s">
+        <v>2558</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>2559</v>
+      </c>
+      <c r="C1166" t="s">
+        <v>2560</v>
+      </c>
+      <c r="D1166" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1166" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:5">
+      <c r="A1167" t="s">
+        <v>2561</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>2563</v>
+      </c>
+      <c r="D1167" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1167" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:5">
+      <c r="A1168" t="s">
+        <v>2564</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>2565</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>2566</v>
+      </c>
+      <c r="D1168" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1168" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:5">
+      <c r="A1169" t="s">
+        <v>2567</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>544</v>
+      </c>
+      <c r="C1169" t="s">
+        <v>2568</v>
+      </c>
+      <c r="D1169" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1169" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:5">
+      <c r="A1170" t="s">
+        <v>2569</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>2570</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>2571</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1170" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:5">
+      <c r="A1171" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>2573</v>
+      </c>
+      <c r="D1171" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1171" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:5">
+      <c r="A1172" t="s">
+        <v>2574</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>2575</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>2576</v>
+      </c>
+      <c r="D1172" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1172" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:5">
+      <c r="A1173" t="s">
+        <v>2577</v>
+      </c>
+      <c r="B1173" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1173" t="s">
+        <v>2578</v>
+      </c>
+      <c r="D1173" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1173" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:5">
+      <c r="A1174" t="s">
+        <v>2579</v>
+      </c>
+      <c r="B1174" t="s">
+        <v>2580</v>
+      </c>
+      <c r="C1174" t="s">
+        <v>2581</v>
+      </c>
+      <c r="D1174" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1174" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:5">
+      <c r="A1175" t="s">
+        <v>2582</v>
+      </c>
+      <c r="B1175" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1175" t="s">
+        <v>2583</v>
+      </c>
+      <c r="D1175" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1175" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:5">
+      <c r="A1176" t="s">
+        <v>2584</v>
+      </c>
+      <c r="B1176" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1176" t="s">
+        <v>2585</v>
+      </c>
+      <c r="D1176" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1176" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:5">
+      <c r="A1177" t="s">
+        <v>2586</v>
+      </c>
+      <c r="B1177" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1177" t="s">
+        <v>2587</v>
+      </c>
+      <c r="D1177" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1177" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:5">
+      <c r="A1178" t="s">
+        <v>2588</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>2589</v>
+      </c>
+      <c r="C1178" t="s">
+        <v>2590</v>
+      </c>
+      <c r="D1178" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1178" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:5">
+      <c r="A1179" t="s">
+        <v>2591</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1179" t="s">
+        <v>2592</v>
+      </c>
+      <c r="D1179" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1179" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:5">
+      <c r="A1180" t="s">
+        <v>2593</v>
+      </c>
+      <c r="B1180" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1180" t="s">
+        <v>2594</v>
+      </c>
+      <c r="D1180" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1180" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:5">
+      <c r="A1181" t="s">
+        <v>2595</v>
+      </c>
+      <c r="B1181" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1181" t="s">
+        <v>2596</v>
+      </c>
+      <c r="D1181" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1181" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:5">
+      <c r="A1182" t="s">
+        <v>2597</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1182" t="s">
+        <v>2598</v>
+      </c>
+      <c r="D1182" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1182" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:5">
+      <c r="A1183" t="s">
+        <v>2599</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1183" t="s">
+        <v>2600</v>
+      </c>
+      <c r="D1183" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1183" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:5">
+      <c r="A1184" t="s">
+        <v>2601</v>
+      </c>
+      <c r="B1184" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1184" t="s">
+        <v>2602</v>
+      </c>
+      <c r="D1184" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1184" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:5">
+      <c r="A1185" t="s">
+        <v>2603</v>
+      </c>
+      <c r="B1185" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1185" t="s">
+        <v>2604</v>
+      </c>
+      <c r="D1185" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1185" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:5">
+      <c r="A1186" t="s">
+        <v>2605</v>
+      </c>
+      <c r="B1186" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1186" t="s">
+        <v>2606</v>
+      </c>
+      <c r="D1186" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1186" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:5">
+      <c r="A1187" t="s">
+        <v>2607</v>
+      </c>
+      <c r="B1187" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1187" t="s">
+        <v>2608</v>
+      </c>
+      <c r="D1187" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1187" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:5">
+      <c r="A1188" t="s">
+        <v>2609</v>
+      </c>
+      <c r="B1188" t="s">
+        <v>2610</v>
+      </c>
+      <c r="C1188" t="s">
+        <v>2611</v>
+      </c>
+      <c r="D1188" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1188" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:5">
+      <c r="A1189" t="s">
+        <v>2612</v>
+      </c>
+      <c r="B1189" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1189" t="s">
+        <v>2613</v>
+      </c>
+      <c r="D1189" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1189" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:5">
+      <c r="A1190" t="s">
+        <v>2614</v>
+      </c>
+      <c r="B1190" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1190" t="s">
+        <v>2615</v>
+      </c>
+      <c r="D1190" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1190" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:5">
+      <c r="A1191" t="s">
+        <v>2616</v>
+      </c>
+      <c r="B1191" t="s">
+        <v>2617</v>
+      </c>
+      <c r="C1191" t="s">
+        <v>2618</v>
+      </c>
+      <c r="D1191" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1191" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:5">
+      <c r="A1192" t="s">
+        <v>2620</v>
+      </c>
+      <c r="B1192" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1192" t="s">
+        <v>2621</v>
+      </c>
+      <c r="D1192" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1192" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:5">
+      <c r="A1193" t="s">
+        <v>2622</v>
+      </c>
+      <c r="B1193" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1193" t="s">
+        <v>2623</v>
+      </c>
+      <c r="D1193" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1193" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:5">
+      <c r="A1194" t="s">
+        <v>2624</v>
+      </c>
+      <c r="B1194" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1194" t="s">
+        <v>2625</v>
+      </c>
+      <c r="D1194" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1194" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:5">
+      <c r="A1195" t="s">
+        <v>2626</v>
+      </c>
+      <c r="B1195" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1195" t="s">
+        <v>2627</v>
+      </c>
+      <c r="D1195" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1195" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:5">
+      <c r="A1196" t="s">
+        <v>2628</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1196" t="s">
+        <v>2629</v>
+      </c>
+      <c r="D1196" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1196" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:5">
+      <c r="A1197" t="s">
+        <v>2630</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1197" t="s">
+        <v>2631</v>
+      </c>
+      <c r="D1197" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1197" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:5">
+      <c r="A1198" t="s">
+        <v>2632</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>518</v>
+      </c>
+      <c r="C1198" t="s">
+        <v>2633</v>
+      </c>
+      <c r="D1198" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1198" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:5">
+      <c r="A1199" t="s">
+        <v>2634</v>
+      </c>
+      <c r="B1199" t="s">
+        <v>2635</v>
+      </c>
+      <c r="C1199" t="s">
+        <v>2636</v>
+      </c>
+      <c r="D1199" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1199" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:5">
+      <c r="A1200" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B1200" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1200" t="s">
+        <v>2638</v>
+      </c>
+      <c r="D1200" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1200" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:5">
+      <c r="A1201" t="s">
+        <v>2639</v>
+      </c>
+      <c r="B1201" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1201" t="s">
+        <v>2640</v>
+      </c>
+      <c r="D1201" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1201" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:5">
+      <c r="A1202" t="s">
+        <v>2641</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C1202" t="s">
+        <v>2642</v>
+      </c>
+      <c r="D1202" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1202" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:5">
+      <c r="A1203" t="s">
+        <v>2643</v>
+      </c>
+      <c r="B1203" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1203" t="s">
+        <v>2644</v>
+      </c>
+      <c r="D1203" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1203" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:5">
+      <c r="A1204" t="s">
+        <v>2645</v>
+      </c>
+      <c r="B1204" t="s">
+        <v>719</v>
+      </c>
+      <c r="C1204" t="s">
+        <v>2646</v>
+      </c>
+      <c r="D1204" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1204" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:5">
+      <c r="A1205" t="s">
+        <v>2647</v>
+      </c>
+      <c r="B1205" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1205" t="s">
+        <v>2648</v>
+      </c>
+      <c r="D1205" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1205" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:5">
+      <c r="A1206" t="s">
+        <v>2649</v>
+      </c>
+      <c r="B1206" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1206" t="s">
+        <v>2650</v>
+      </c>
+      <c r="D1206" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1206" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:5">
+      <c r="A1207" t="s">
+        <v>2651</v>
+      </c>
+      <c r="B1207" t="s">
+        <v>518</v>
+      </c>
+      <c r="C1207" t="s">
+        <v>2652</v>
+      </c>
+      <c r="D1207" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1207" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:5">
+      <c r="A1208" t="s">
+        <v>2653</v>
+      </c>
+      <c r="B1208" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1208" t="s">
+        <v>2654</v>
+      </c>
+      <c r="D1208" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1208" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:5">
+      <c r="A1209" t="s">
+        <v>2655</v>
+      </c>
+      <c r="B1209" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1209" t="s">
+        <v>2656</v>
+      </c>
+      <c r="D1209" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1209" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:5">
+      <c r="A1210" t="s">
+        <v>2657</v>
+      </c>
+      <c r="B1210" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1210" t="s">
+        <v>2658</v>
+      </c>
+      <c r="D1210" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1210" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:5">
+      <c r="A1211" t="s">
+        <v>2659</v>
+      </c>
+      <c r="B1211" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1211" t="s">
+        <v>2660</v>
+      </c>
+      <c r="D1211" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1211" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:5">
+      <c r="A1212" t="s">
+        <v>2661</v>
+      </c>
+      <c r="B1212" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1212" t="s">
+        <v>2662</v>
+      </c>
+      <c r="D1212" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1212" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:5">
+      <c r="A1213" t="s">
+        <v>2663</v>
+      </c>
+      <c r="B1213" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1213" t="s">
+        <v>2664</v>
+      </c>
+      <c r="D1213" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1213" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:5">
+      <c r="A1214" t="s">
+        <v>2665</v>
+      </c>
+      <c r="B1214" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1214" t="s">
+        <v>2666</v>
+      </c>
+      <c r="D1214" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1214" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:5">
+      <c r="A1215" t="s">
+        <v>2667</v>
+      </c>
+      <c r="B1215" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1215" t="s">
+        <v>2668</v>
+      </c>
+      <c r="D1215" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1215" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:5">
+      <c r="A1216" t="s">
+        <v>2669</v>
+      </c>
+      <c r="B1216" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1216" t="s">
+        <v>2670</v>
+      </c>
+      <c r="D1216" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1216" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:5">
+      <c r="A1217" t="s">
+        <v>2671</v>
+      </c>
+      <c r="B1217" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1217" t="s">
+        <v>2672</v>
+      </c>
+      <c r="D1217" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1217" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:5">
+      <c r="A1218" t="s">
+        <v>2673</v>
+      </c>
+      <c r="B1218" t="s">
+        <v>2461</v>
+      </c>
+      <c r="C1218" t="s">
+        <v>2674</v>
+      </c>
+      <c r="D1218" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1218" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:5">
+      <c r="A1219" t="s">
+        <v>2675</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1219" t="s">
+        <v>2676</v>
+      </c>
+      <c r="D1219" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1219" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:5">
+      <c r="A1220" t="s">
+        <v>2677</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1220" t="s">
+        <v>2678</v>
+      </c>
+      <c r="D1220" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1220" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:5">
+      <c r="A1221" t="s">
+        <v>2679</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1221" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D1221" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1221" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:5">
+      <c r="A1222" t="s">
+        <v>2681</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1222" t="s">
+        <v>2682</v>
+      </c>
+      <c r="D1222" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1222" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:5">
+      <c r="A1223" t="s">
+        <v>2683</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1223" t="s">
+        <v>2684</v>
+      </c>
+      <c r="D1223" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1223" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:5">
+      <c r="A1224" t="s">
+        <v>2685</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>953</v>
+      </c>
+      <c r="C1224" t="s">
+        <v>2686</v>
+      </c>
+      <c r="D1224" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1224" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:5">
+      <c r="A1225" t="s">
+        <v>2687</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1225" t="s">
+        <v>2688</v>
+      </c>
+      <c r="D1225" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1225" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:5">
+      <c r="A1226" t="s">
+        <v>2689</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1226" t="s">
+        <v>2690</v>
+      </c>
+      <c r="D1226" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1226" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:5">
+      <c r="A1227" t="s">
+        <v>2691</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1227" t="s">
+        <v>2692</v>
+      </c>
+      <c r="D1227" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1227" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:5">
+      <c r="A1228" t="s">
+        <v>2693</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>573</v>
+      </c>
+      <c r="C1228" t="s">
+        <v>2694</v>
+      </c>
+      <c r="D1228" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1228" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:5">
+      <c r="A1229" t="s">
+        <v>2695</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1229" t="s">
+        <v>2696</v>
+      </c>
+      <c r="D1229" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1229" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:5">
+      <c r="A1230" t="s">
+        <v>2697</v>
+      </c>
+      <c r="B1230" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1230" t="s">
+        <v>2698</v>
+      </c>
+      <c r="D1230" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1230" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:5">
+      <c r="A1231" t="s">
+        <v>2699</v>
+      </c>
+      <c r="B1231" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1231" t="s">
+        <v>2700</v>
+      </c>
+      <c r="D1231" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1231" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:5">
+      <c r="A1232" t="s">
+        <v>2701</v>
+      </c>
+      <c r="B1232" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1232" t="s">
+        <v>2702</v>
+      </c>
+      <c r="D1232" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1232" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:5">
+      <c r="A1233" t="s">
+        <v>2703</v>
+      </c>
+      <c r="B1233" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1233" t="s">
+        <v>2704</v>
+      </c>
+      <c r="D1233" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1233" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:5">
+      <c r="A1234" t="s">
+        <v>2705</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>2706</v>
+      </c>
+      <c r="C1234" t="s">
+        <v>2707</v>
+      </c>
+      <c r="D1234" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1234" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:5">
+      <c r="A1235" t="s">
+        <v>2708</v>
+      </c>
+      <c r="B1235" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C1235" t="s">
+        <v>2709</v>
+      </c>
+      <c r="D1235" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1235" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:5">
+      <c r="A1236" t="s">
+        <v>2710</v>
+      </c>
+      <c r="B1236" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1236" t="s">
+        <v>2711</v>
+      </c>
+      <c r="D1236" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1236" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:5">
+      <c r="A1237" t="s">
+        <v>2712</v>
+      </c>
+      <c r="B1237" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1237" t="s">
+        <v>2713</v>
+      </c>
+      <c r="D1237" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1237" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:5">
+      <c r="A1238" t="s">
+        <v>2714</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1238" t="s">
+        <v>2715</v>
+      </c>
+      <c r="D1238" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1238" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:5">
+      <c r="A1239" t="s">
+        <v>2716</v>
+      </c>
+      <c r="B1239" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1239" t="s">
+        <v>2717</v>
+      </c>
+      <c r="D1239" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1239" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:5">
+      <c r="A1240" t="s">
+        <v>2718</v>
+      </c>
+      <c r="B1240" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1240" t="s">
+        <v>2719</v>
+      </c>
+      <c r="D1240" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1240" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:5">
+      <c r="A1241" t="s">
+        <v>2720</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1241" t="s">
+        <v>2721</v>
+      </c>
+      <c r="D1241" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1241" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:5">
+      <c r="A1242" t="s">
+        <v>2722</v>
+      </c>
+      <c r="B1242" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1242" t="s">
+        <v>2723</v>
+      </c>
+      <c r="D1242" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1242" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:5">
+      <c r="A1243" t="s">
+        <v>2724</v>
+      </c>
+      <c r="B1243" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1243" t="s">
+        <v>2725</v>
+      </c>
+      <c r="D1243" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1243" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:5">
+      <c r="A1244" t="s">
+        <v>2726</v>
+      </c>
+      <c r="B1244" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1244" t="s">
+        <v>2727</v>
+      </c>
+      <c r="D1244" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1244" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:5">
+      <c r="A1245" t="s">
+        <v>2728</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1245" t="s">
+        <v>2729</v>
+      </c>
+      <c r="D1245" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1245" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:5">
+      <c r="A1246" t="s">
+        <v>2730</v>
+      </c>
+      <c r="B1246" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1246" t="s">
+        <v>2731</v>
+      </c>
+      <c r="D1246" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1246" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:5">
+      <c r="A1247" t="s">
+        <v>2732</v>
+      </c>
+      <c r="B1247" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1247" t="s">
+        <v>2733</v>
+      </c>
+      <c r="D1247" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1247" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:5">
+      <c r="A1248" t="s">
+        <v>2734</v>
+      </c>
+      <c r="B1248" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1248" t="s">
+        <v>2735</v>
+      </c>
+      <c r="D1248" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1248" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:5">
+      <c r="A1249" t="s">
+        <v>2736</v>
+      </c>
+      <c r="B1249" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1249" t="s">
+        <v>2737</v>
+      </c>
+      <c r="D1249" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1249" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:5">
+      <c r="A1250" t="s">
+        <v>2738</v>
+      </c>
+      <c r="B1250" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1250" t="s">
+        <v>2739</v>
+      </c>
+      <c r="D1250" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1250" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:5">
+      <c r="A1251" t="s">
+        <v>2740</v>
+      </c>
+      <c r="B1251" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1251" t="s">
+        <v>2741</v>
+      </c>
+      <c r="D1251" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1251" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:5">
+      <c r="A1252" t="s">
+        <v>2742</v>
+      </c>
+      <c r="B1252" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C1252" t="s">
+        <v>2743</v>
+      </c>
+      <c r="D1252" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1252" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:5">
+      <c r="A1253" t="s">
+        <v>2744</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1253" t="s">
+        <v>2745</v>
+      </c>
+      <c r="D1253" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1253" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:5">
+      <c r="A1254" t="s">
+        <v>2746</v>
+      </c>
+      <c r="B1254" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1254" t="s">
+        <v>2747</v>
+      </c>
+      <c r="D1254" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1254" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:5">
+      <c r="A1255" t="s">
+        <v>2748</v>
+      </c>
+      <c r="B1255" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1255" t="s">
+        <v>2749</v>
+      </c>
+      <c r="D1255" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1255" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:5">
+      <c r="A1256" t="s">
+        <v>2750</v>
+      </c>
+      <c r="B1256" t="s">
+        <v>2751</v>
+      </c>
+      <c r="C1256" t="s">
+        <v>2752</v>
+      </c>
+      <c r="D1256" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1256" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:5">
+      <c r="A1257" t="s">
+        <v>2753</v>
+      </c>
+      <c r="B1257" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1257" t="s">
+        <v>2754</v>
+      </c>
+      <c r="D1257" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1257" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:5">
+      <c r="A1258" t="s">
+        <v>2755</v>
+      </c>
+      <c r="B1258" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1258" t="s">
+        <v>2756</v>
+      </c>
+      <c r="D1258" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1258" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:5">
+      <c r="A1259" t="s">
+        <v>2757</v>
+      </c>
+      <c r="B1259" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1259" t="s">
+        <v>2758</v>
+      </c>
+      <c r="D1259" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1259" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:5">
+      <c r="A1260" t="s">
+        <v>2759</v>
+      </c>
+      <c r="B1260" t="s">
+        <v>544</v>
+      </c>
+      <c r="C1260" t="s">
+        <v>2760</v>
+      </c>
+      <c r="D1260" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1260" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:5">
+      <c r="A1261" t="s">
+        <v>2761</v>
+      </c>
+      <c r="B1261" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1261" t="s">
+        <v>2762</v>
+      </c>
+      <c r="D1261" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1261" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:5">
+      <c r="A1262" t="s">
+        <v>2763</v>
+      </c>
+      <c r="B1262" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1262" t="s">
+        <v>2764</v>
+      </c>
+      <c r="D1262" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1262" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:5">
+      <c r="A1263" t="s">
+        <v>2765</v>
+      </c>
+      <c r="B1263" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1263" t="s">
+        <v>2766</v>
+      </c>
+      <c r="D1263" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1263" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:5">
+      <c r="A1264" t="s">
+        <v>2767</v>
+      </c>
+      <c r="B1264" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1264" t="s">
+        <v>2768</v>
+      </c>
+      <c r="D1264" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1264" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:5">
+      <c r="A1265" t="s">
+        <v>2769</v>
+      </c>
+      <c r="B1265" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1265" t="s">
+        <v>2770</v>
+      </c>
+      <c r="D1265" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1265" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:5">
+      <c r="A1266" t="s">
+        <v>2771</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1266" t="s">
+        <v>2772</v>
+      </c>
+      <c r="D1266" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1266" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:5">
+      <c r="A1267" t="s">
+        <v>2773</v>
+      </c>
+      <c r="B1267" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1267" t="s">
+        <v>2774</v>
+      </c>
+      <c r="D1267" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1267" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:5">
+      <c r="A1268" t="s">
+        <v>2775</v>
+      </c>
+      <c r="B1268" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1268" t="s">
+        <v>2776</v>
+      </c>
+      <c r="D1268" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1268" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:5">
+      <c r="A1269" t="s">
+        <v>2777</v>
+      </c>
+      <c r="B1269" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1269" t="s">
+        <v>2778</v>
+      </c>
+      <c r="D1269" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1269" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:5">
+      <c r="A1270" t="s">
+        <v>2779</v>
+      </c>
+      <c r="B1270" t="s">
+        <v>2780</v>
+      </c>
+      <c r="C1270" t="s">
+        <v>2781</v>
+      </c>
+      <c r="D1270" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1270" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:5">
+      <c r="A1271" t="s">
+        <v>2782</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1271" t="s">
+        <v>2783</v>
+      </c>
+      <c r="D1271" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1271" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:5">
+      <c r="A1272" t="s">
+        <v>2784</v>
+      </c>
+      <c r="B1272" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1272" t="s">
+        <v>2785</v>
+      </c>
+      <c r="D1272" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1272" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:5">
+      <c r="A1273" t="s">
+        <v>2786</v>
+      </c>
+      <c r="B1273" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1273" t="s">
+        <v>2787</v>
+      </c>
+      <c r="D1273" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1273" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:5">
+      <c r="A1274" t="s">
+        <v>2788</v>
+      </c>
+      <c r="B1274" t="s">
+        <v>2789</v>
+      </c>
+      <c r="C1274" t="s">
+        <v>2790</v>
+      </c>
+      <c r="D1274" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1274" t="s">
+        <v>2791</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:5">
+      <c r="A1275" t="s">
+        <v>2792</v>
+      </c>
+      <c r="B1275" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1275" t="s">
+        <v>2793</v>
+      </c>
+      <c r="D1275" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1275" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:5">
+      <c r="A1276" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B1276" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1276" t="s">
+        <v>2795</v>
+      </c>
+      <c r="D1276" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1276" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:5">
+      <c r="A1277" t="s">
+        <v>2796</v>
+      </c>
+      <c r="B1277" t="s">
+        <v>2797</v>
+      </c>
+      <c r="C1277" t="s">
+        <v>2798</v>
+      </c>
+      <c r="D1277" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1277" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:5">
+      <c r="A1278" t="s">
+        <v>2799</v>
+      </c>
+      <c r="B1278" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1278" t="s">
+        <v>2800</v>
+      </c>
+      <c r="D1278" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1278" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:5">
+      <c r="A1279" t="s">
+        <v>2801</v>
+      </c>
+      <c r="B1279" t="s">
+        <v>2802</v>
+      </c>
+      <c r="C1279" t="s">
+        <v>2803</v>
+      </c>
+      <c r="D1279" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1279" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:5">
+      <c r="A1280" t="s">
+        <v>2804</v>
+      </c>
+      <c r="B1280" t="s">
+        <v>832</v>
+      </c>
+      <c r="C1280" t="s">
+        <v>2805</v>
+      </c>
+      <c r="D1280" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1280" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:5">
+      <c r="A1281" t="s">
+        <v>2806</v>
+      </c>
+      <c r="B1281" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1281" t="s">
+        <v>2807</v>
+      </c>
+      <c r="D1281" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1281" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:5">
+      <c r="A1282" t="s">
+        <v>2808</v>
+      </c>
+      <c r="B1282" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1282" t="s">
+        <v>2809</v>
+      </c>
+      <c r="D1282" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1282" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:5">
+      <c r="A1283" t="s">
+        <v>2810</v>
+      </c>
+      <c r="B1283" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1283" t="s">
+        <v>2811</v>
+      </c>
+      <c r="D1283" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1283" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:5">
+      <c r="A1284" t="s">
+        <v>2812</v>
+      </c>
+      <c r="B1284" t="s">
+        <v>544</v>
+      </c>
+      <c r="C1284" t="s">
+        <v>2813</v>
+      </c>
+      <c r="D1284" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1284" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:5">
+      <c r="A1285" t="s">
+        <v>2814</v>
+      </c>
+      <c r="B1285" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1285" t="s">
+        <v>2815</v>
+      </c>
+      <c r="D1285" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1285" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:5">
+      <c r="A1286" t="s">
+        <v>2816</v>
+      </c>
+      <c r="B1286" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1286" t="s">
+        <v>2817</v>
+      </c>
+      <c r="D1286" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1286" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:5">
+      <c r="A1287" t="s">
+        <v>2818</v>
+      </c>
+      <c r="B1287" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1287" t="s">
+        <v>2819</v>
+      </c>
+      <c r="D1287" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1287" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:5">
+      <c r="A1288" t="s">
+        <v>2820</v>
+      </c>
+      <c r="B1288" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1288" t="s">
+        <v>2821</v>
+      </c>
+      <c r="D1288" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1288" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:5">
+      <c r="A1289" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B1289" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1289" t="s">
+        <v>2823</v>
+      </c>
+      <c r="D1289" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1289" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:5">
+      <c r="A1290" t="s">
+        <v>2824</v>
+      </c>
+      <c r="B1290" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1290" t="s">
+        <v>2825</v>
+      </c>
+      <c r="D1290" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1290" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:5">
+      <c r="A1291" t="s">
+        <v>2826</v>
+      </c>
+      <c r="B1291" t="s">
+        <v>446</v>
+      </c>
+      <c r="C1291" t="s">
+        <v>2827</v>
+      </c>
+      <c r="D1291" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1291" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:5">
+      <c r="A1292" t="s">
+        <v>2828</v>
+      </c>
+      <c r="B1292" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1292" t="s">
+        <v>2829</v>
+      </c>
+      <c r="D1292" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1292" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:5">
+      <c r="A1293" t="s">
+        <v>2830</v>
+      </c>
+      <c r="B1293" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C1293" t="s">
+        <v>2831</v>
+      </c>
+      <c r="D1293" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1293" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:5">
+      <c r="A1294" t="s">
+        <v>2832</v>
+      </c>
+      <c r="B1294" t="s">
+        <v>832</v>
+      </c>
+      <c r="C1294" t="s">
+        <v>2833</v>
+      </c>
+      <c r="D1294" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1294" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:5">
+      <c r="A1295" t="s">
+        <v>2834</v>
+      </c>
+      <c r="B1295" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1295" t="s">
+        <v>2835</v>
+      </c>
+      <c r="D1295" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1295" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:5">
+      <c r="A1296" t="s">
+        <v>2836</v>
+      </c>
+      <c r="B1296" t="s">
+        <v>832</v>
+      </c>
+      <c r="C1296" t="s">
+        <v>2837</v>
+      </c>
+      <c r="D1296" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1296" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:5">
+      <c r="A1297" t="s">
+        <v>2838</v>
+      </c>
+      <c r="B1297" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1297" t="s">
+        <v>2839</v>
+      </c>
+      <c r="D1297" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1297" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:5">
+      <c r="A1298" t="s">
+        <v>2840</v>
+      </c>
+      <c r="B1298" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1298" t="s">
+        <v>2841</v>
+      </c>
+      <c r="D1298" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1298" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:5">
+      <c r="A1299" t="s">
+        <v>2842</v>
+      </c>
+      <c r="B1299" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1299" t="s">
+        <v>2843</v>
+      </c>
+      <c r="D1299" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1299" t="s">
+        <v>2844</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:5">
+      <c r="A1300" t="s">
+        <v>2845</v>
+      </c>
+      <c r="B1300" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1300" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D1300" t="s">
+        <v>634</v>
+      </c>
+      <c r="E1300" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:5">
+      <c r="A1301" t="s">
+        <v>2847</v>
+      </c>
+      <c r="B1301" t="s">
+        <v>2848</v>
+      </c>
+      <c r="C1301" t="s">
+        <v>2849</v>
+      </c>
+      <c r="D1301" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1301" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>